<commit_message>
Analisis de F1 Score
</commit_message>
<xml_diff>
--- a/documentation/analisis_resultados.xlsx
+++ b/documentation/analisis_resultados.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEC\2018IISemestre\IA\Proyecto1-IA-Cancer-Predictions\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TEC\2018IISemestre\IA\Proyecto1-IA-Cancer-Predictions\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Arbol - Porcentaje de pruebas " sheetId="1" r:id="rId1"/>
     <sheet name="Arbol - Poda" sheetId="2" r:id="rId2"/>
     <sheet name="Redes - Capas y Unidades" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparación Modelos" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>err ent poda</t>
   </si>
@@ -125,6 +126,36 @@
   </si>
   <si>
     <t>6 &gt; 20</t>
+  </si>
+  <si>
+    <t>Exhaustividad</t>
+  </si>
+  <si>
+    <t>Precisión</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>F1 Custom</t>
+  </si>
+  <si>
+    <t>Random forest</t>
+  </si>
+  <si>
+    <t>Redes</t>
+  </si>
+  <si>
+    <t>Promedio Exh</t>
+  </si>
+  <si>
+    <t>Promedio Precision</t>
+  </si>
+  <si>
+    <t>Promedio F1 Score</t>
+  </si>
+  <si>
+    <t>Promedio F1 Custom</t>
   </si>
 </sst>
 </file>
@@ -304,7 +335,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -318,6 +349,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Énfasis1" xfId="4" builtinId="31"/>
@@ -4522,7 +4554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -6188,4 +6220,454 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.97629999999999995</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.97389999999999999</v>
+      </c>
+      <c r="E3" s="3">
+        <f>(B3*B3*C3*2)/(B3+C3)</f>
+        <v>0.94628431082499109</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="3">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.96644999999999981</v>
+      </c>
+      <c r="J3" s="13">
+        <f>AVERAGE(B14:B23)</f>
+        <v>0.97354000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.96689999999999998</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E23" si="0">(B4*B4*C4*2)/(B4+C4)</f>
+        <v>0.9506285118714729</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="3">
+        <f>AVERAGE(C3:C12)</f>
+        <v>0.97785999999999995</v>
+      </c>
+      <c r="J4" s="13">
+        <f>AVERAGE(C14:C23)</f>
+        <v>0.98429999999999984</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.95750000000000002</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.995</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.97589999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.9344145646606915</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3">
+        <f>AVERAGE(D3:D12)</f>
+        <v>0.97198799999999996</v>
+      </c>
+      <c r="J5" s="13">
+        <f>AVERAGE(D14:D23)</f>
+        <v>0.97884999999999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.96689999999999998</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.95340000000000003</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.96018000000000003</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.92832315218872052</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="3">
+        <f>AVERAGE(E3:E12)</f>
+        <v>0.9394243516268137</v>
+      </c>
+      <c r="J6" s="13">
+        <f>AVERAGE(E14:E23)</f>
+        <v>0.95296305070609344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.95528644720191191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.94950000000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.9627</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.94004095074510641</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.97650000000000003</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.9788</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.9602953775694727</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.98009999999999997</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.89322157024137927</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.96220000000000006</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.98550000000000004</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.97370000000000001</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.93690437112491654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.96719999999999995</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.9718</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.94884425983947329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.99039999999999995</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.9601431087899126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="13">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.98089999999999999</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95300443077424946</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="13">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95559740243179736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="13">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.97189999999999999</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.97650000000000003</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95802289032155652</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="13">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.98560000000000003</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95075911050071538</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>6</v>
+      </c>
+      <c r="B19" s="13">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.9718</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.97409999999999997</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95110593750949612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>7</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.97640000000000005</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95335696000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>8</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.97160000000000002</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.98319999999999996</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95528644720191191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>9</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.95279999999999998</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.97109999999999996</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.92525641503319778</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>10</v>
+      </c>
+      <c r="B23" s="13">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.99039999999999995</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.98570000000000002</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>0.9670978044980979</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>